<commit_message>
add changes in import
</commit_message>
<xml_diff>
--- a/formatos upload/alumno.xlsx
+++ b/formatos upload/alumno.xlsx
@@ -24,126 +24,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
-  <si>
-    <t>00002</t>
-  </si>
-  <si>
-    <t>00003</t>
-  </si>
-  <si>
-    <t>00004</t>
-  </si>
-  <si>
-    <t>00005</t>
-  </si>
-  <si>
-    <t>00006</t>
-  </si>
-  <si>
-    <t>00007</t>
-  </si>
-  <si>
-    <t>00008</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>CODIGO ESCUELA</t>
   </si>
   <si>
-    <t>00001</t>
-  </si>
-  <si>
-    <t>00099</t>
-  </si>
-  <si>
     <t>NOMBRES</t>
   </si>
   <si>
     <t>APELLIDOS</t>
   </si>
   <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Perez Perez</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Ponce Bellido</t>
-  </si>
-  <si>
-    <t>Carlos Martin</t>
-  </si>
-  <si>
-    <t>Gonzales Prado</t>
-  </si>
-  <si>
-    <t>Pacheco Duran</t>
-  </si>
-  <si>
-    <t>Hernan Jose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vilma </t>
-  </si>
-  <si>
-    <t>Flores Ramos</t>
-  </si>
-  <si>
-    <t>Andrea</t>
-  </si>
-  <si>
-    <t>Alvia</t>
-  </si>
-  <si>
-    <t>Carbajal Camposano</t>
-  </si>
-  <si>
-    <t>Luz</t>
-  </si>
-  <si>
-    <t>Caldas Torrejon</t>
-  </si>
-  <si>
     <t>USUARIO</t>
   </si>
   <si>
     <t>EMAIL</t>
   </si>
   <si>
-    <t>jperez@gmail.com</t>
-  </si>
-  <si>
-    <t>mponce@gmail.com</t>
-  </si>
-  <si>
-    <t>cgonzales@gmail.com</t>
-  </si>
-  <si>
-    <t>hpacheco@gmail.com</t>
-  </si>
-  <si>
-    <t>vflores@gmail.com</t>
-  </si>
-  <si>
-    <t>anuñez@gmail.com</t>
-  </si>
-  <si>
-    <t>acarbajal@gmail.com</t>
-  </si>
-  <si>
-    <t>lcaldas@gmail.com</t>
-  </si>
-  <si>
-    <t>Nuñez Carbajal</t>
-  </si>
-  <si>
     <t>CODIGO ALUMNO</t>
   </si>
   <si>
     <t>AÑO INGRESO</t>
+  </si>
+  <si>
+    <t>Edinson</t>
+  </si>
+  <si>
+    <t>Nuñez More</t>
+  </si>
+  <si>
+    <t>nmedinson@gmail.com</t>
+  </si>
+  <si>
+    <t>42853598</t>
+  </si>
+  <si>
+    <t>000001</t>
   </si>
 </sst>
 </file>
@@ -495,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,223 +429,55 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="E2">
         <v>2001</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>2002</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4">
-        <v>20003</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5">
-        <v>2005</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6">
-        <v>2001</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7">
-        <v>2000</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8">
-        <v>2006</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9">
-        <v>2009</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
-    <hyperlink ref="G8" r:id="rId7"/>
-    <hyperlink ref="G9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>